<commit_message>
presentation plus physics record updated
</commit_message>
<xml_diff>
--- a/Semester_4/PHY212/Analysis/Experiment_4/exp4.xlsx
+++ b/Semester_4/PHY212/Analysis/Experiment_4/exp4.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14128"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A. S. Aurora\Documents\IISER_repo\Semester_4\PHY212\Analysis\Experiment_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atul\Documents\IISER_repo\Semester_4\PHY212\Analysis\Experiment_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -108,8 +111,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -346,11 +377,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="228718688"/>
-        <c:axId val="228719072"/>
+        <c:axId val="1108014704"/>
+        <c:axId val="1575816672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="228718688"/>
+        <c:axId val="1108014704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -407,12 +438,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228719072"/>
+        <c:crossAx val="1575816672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="228719072"/>
+        <c:axId val="1575816672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -469,7 +500,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228718688"/>
+        <c:crossAx val="1108014704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -710,11 +741,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="228870256"/>
-        <c:axId val="228823928"/>
+        <c:axId val="1575829184"/>
+        <c:axId val="1575819936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="228870256"/>
+        <c:axId val="1575829184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -766,12 +797,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228823928"/>
+        <c:crossAx val="1575819936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="228823928"/>
+        <c:axId val="1575819936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -827,7 +858,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228870256"/>
+        <c:crossAx val="1575829184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1071,11 +1102,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="228832504"/>
-        <c:axId val="229985664"/>
+        <c:axId val="1575819392"/>
+        <c:axId val="1575823200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="228832504"/>
+        <c:axId val="1575819392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1127,12 +1158,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229985664"/>
+        <c:crossAx val="1575823200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="229985664"/>
+        <c:axId val="1575823200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1188,7 +1219,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228832504"/>
+        <c:crossAx val="1575819392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1255,6 +1286,30 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>2M</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1408,11 +1463,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="229116512"/>
-        <c:axId val="229116896"/>
+        <c:axId val="1575821024"/>
+        <c:axId val="1575817760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="229116512"/>
+        <c:axId val="1575821024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1464,12 +1519,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229116896"/>
+        <c:crossAx val="1575817760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="229116896"/>
+        <c:axId val="1575817760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1525,7 +1580,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229116512"/>
+        <c:crossAx val="1575821024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3873,16 +3928,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>261937</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>80962</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>566737</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>385762</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3908,16 +3963,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3938,16 +3993,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3968,16 +4023,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4045,12 +4100,47 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Tahoma"/>
-        <a:font script="Hebr" typeface="Gisha"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
         <a:font script="Thai" typeface="Tahoma"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
@@ -4072,42 +4162,7 @@
         <a:font script="Laoo" typeface="DokChampa"/>
         <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Tahoma"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Tahoma"/>
-        <a:font script="Hebr" typeface="Gisha"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Verdana"/>
+        <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
@@ -4264,8 +4319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4411,16 +4466,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4430,7 +4486,7 @@
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4455,11 +4511,11 @@
       <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -4482,7 +4538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>609</v>
       </c>
@@ -4507,11 +4563,11 @@
         <f t="shared" ref="H3:H8" si="2">D$2-D3</f>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>514</v>
       </c>
@@ -4537,7 +4593,7 @@
         <v>4.3000000000000038E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>438</v>
       </c>
@@ -4563,7 +4619,7 @@
         <v>3.1000000000000028E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>274</v>
       </c>
@@ -4589,7 +4645,7 @@
         <v>2.1000000000000019E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>168</v>
       </c>
@@ -4615,7 +4671,7 @@
         <v>1.100000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>16</v>
       </c>
@@ -4641,7 +4697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>0</v>
       </c>
@@ -4655,7 +4711,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>12</v>
       </c>
@@ -4678,7 +4734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>614</v>
       </c>
@@ -4704,7 +4760,7 @@
         <v>3.7000000000000033E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>547</v>
       </c>
@@ -4730,7 +4786,7 @@
         <v>3.1000000000000028E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>431</v>
       </c>
@@ -4756,7 +4812,7 @@
         <v>2.5000000000000022E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>328</v>
       </c>
@@ -4782,7 +4838,7 @@
         <v>1.9000000000000017E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>193</v>
       </c>
@@ -4808,7 +4864,7 @@
         <v>1.6000000000000014E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>96</v>
       </c>
@@ -5169,6 +5225,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>